<commit_message>
BE : WIP itemizer: Todo Rip Measurement
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2AE87A-55BA-437D-A792-30C4DFAAB772}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119BD197-A62C-4314-9D15-E00D9324AAC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13455" yWindow="4200" windowWidth="26490" windowHeight="24525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="4545" windowWidth="26490" windowHeight="24525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
+    <sheet name="Synth" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$H$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="20" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>EWIN SERVICES</t>
   </si>
@@ -41,7 +45,52 @@
     <t>Partenaire</t>
   </si>
   <si>
-    <t>header</t>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Code BPU</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Prix</t>
+  </si>
+  <si>
+    <t>Installé</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Étiquettes de lignes</t>
+  </si>
+  <si>
+    <t>(vide)</t>
+  </si>
+  <si>
+    <t>Total général</t>
+  </si>
+  <si>
+    <t>Étiquettes de colonnes</t>
+  </si>
+  <si>
+    <t>Somme de Quantité</t>
+  </si>
+  <si>
+    <t>Total Somme de Quantité</t>
+  </si>
+  <si>
+    <t>Total Somme de Prix</t>
+  </si>
+  <si>
+    <t>Somme de Prix</t>
   </si>
 </sst>
 </file>
@@ -113,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -132,6 +181,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -203,6 +257,133 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent" refreshedDate="43610.853990162039" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{A18E6F46-E4AC-43A0-BEA1-2DC454C5FF12}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A9:H1009" sheet="EWIN"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Item" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Info" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Code BPU" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Quantité" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Prix" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Installé" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Equipe" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="165">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB490DDA-5D40-492A-B43F-98E467069B29}" name="Tableau croisé dynamique3" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:E7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="5"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Somme de Quantité" fld="3" baseField="2" baseItem="0"/>
+    <dataField name="Somme de Prix" fld="4" baseField="2" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,7 +652,7 @@
   <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,25 +689,25 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -535,4 +716,71 @@
   <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35326CA-C26B-42CB-A6C3-92DFEFAA53AC}">
+  <dimension ref="A3:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BE + FE : Rip Stat MVP
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119BD197-A62C-4314-9D15-E00D9324AAC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FEED0B-FE95-43A5-B788-111FE9BC4EAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="4545" windowWidth="26490" windowHeight="24525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="3945" windowWidth="26490" windowHeight="24525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
     <sheet name="Synth" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$H$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$J$243</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>EWIN SERVICES</t>
   </si>
@@ -91,15 +91,22 @@
   </si>
   <si>
     <t>Somme de Prix</t>
+  </si>
+  <si>
+    <t>Quant. Tr.</t>
+  </si>
+  <si>
+    <t>Travail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -167,16 +174,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +184,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,16 +221,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>71158</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>112705</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309283</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>150804</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -246,7 +259,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11306175" y="209551"/>
+          <a:off x="57150" y="57150"/>
           <a:ext cx="1499908" cy="855654"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -260,7 +273,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent" refreshedDate="43610.853990162039" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{A18E6F46-E4AC-43A0-BEA1-2DC454C5FF12}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43610.853990162039" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{A18E6F46-E4AC-43A0-BEA1-2DC454C5FF12}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:H1009" sheet="EWIN"/>
   </cacheSource>
@@ -318,7 +331,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB490DDA-5D40-492A-B43F-98E467069B29}" name="Tableau croisé dynamique3" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB490DDA-5D40-492A-B43F-98E467069B29}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -648,8 +661,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A1274-8C24-433A-8202-5D2FE710C049}">
+  <dimension ref="A2:J9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -659,19 +672,19 @@
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="14" customWidth="1"/>
     <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I2" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -680,38 +693,47 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="I9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="J9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A9:H9" xr:uid="{A9D4A1A4-C41E-4E7C-832B-26A8197C1889}"/>
+  <autoFilter ref="A9:J243" xr:uid="{A0DF9817-DEF9-461E-807D-932DE473B341}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -719,11 +741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35326CA-C26B-42CB-A6C3-92DFEFAA53AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D00292-05A1-482C-9067-25F908AE77CB}">
   <dimension ref="A3:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +758,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -752,7 +774,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -763,22 +785,22 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BE: Fix Underground activity typo + Attachment XLS file
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FEED0B-FE95-43A5-B788-111FE9BC4EAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F833152-DD8E-40AE-8810-8D6B479DE9A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="3945" windowWidth="26490" windowHeight="24525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16545" yWindow="6330" windowWidth="31245" windowHeight="22965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -273,11 +273,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43610.853990162039" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{A18E6F46-E4AC-43A0-BEA1-2DC454C5FF12}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43659.490395949077" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{4E7DB3FF-3921-4F05-9A1D-32673DE941C7}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A9:H1009" sheet="EWIN"/>
+    <worksheetSource ref="A9:J1009" sheet="EWIN"/>
   </cacheSource>
-  <cacheFields count="8">
+  <cacheFields count="10">
     <cacheField name="Item" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -295,7 +295,13 @@
     <cacheField name="Prix" numFmtId="164">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Installé" numFmtId="0">
+    <cacheField name="Quant. Tr." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Travail" numFmtId="166">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Installé" numFmtId="165">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
         <m/>
       </sharedItems>
@@ -303,7 +309,7 @@
     <cacheField name="Equipe" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Date" numFmtId="165">
+    <cacheField name="Date" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -323,6 +329,8 @@
     <x v="0"/>
     <m/>
     <m/>
+    <m/>
+    <m/>
     <x v="0"/>
     <m/>
     <m/>
@@ -331,12 +339,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB490DDA-5D40-492A-B43F-98E467069B29}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86E8B809-2561-47F1-B5BD-247667BDDFCB}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="8">
+  <pivotFields count="10">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
@@ -344,6 +352,8 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -365,7 +375,7 @@
     </i>
   </rowItems>
   <colFields count="2">
-    <field x="5"/>
+    <field x="7"/>
     <field x="-2"/>
   </colFields>
   <colItems count="4">
@@ -664,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A1274-8C24-433A-8202-5D2FE710C049}">
   <dimension ref="A2:J9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -744,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D00292-05A1-482C-9067-25F908AE77CB}">
   <dimension ref="A3:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BE+FE Pole Itemize completed and Pole Attachement Route done
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F833152-DD8E-40AE-8810-8D6B479DE9A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40997A8F-8816-4FFE-8B19-128A95FF8AFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16545" yWindow="6330" windowWidth="31245" windowHeight="22965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9915" yWindow="6690" windowWidth="36750" windowHeight="21030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -169,9 +169,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -198,6 +197,18 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -273,7 +284,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43659.490395949077" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{4E7DB3FF-3921-4F05-9A1D-32673DE941C7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43693.783743055559" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{4E7DB3FF-3921-4F05-9A1D-32673DE941C7}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:J1009" sheet="EWIN"/>
   </cacheSource>
@@ -339,7 +350,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86E8B809-2561-47F1-B5BD-247667BDDFCB}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86E8B809-2561-47F1-B5BD-247667BDDFCB}" name="Tableau croisé dynamique3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -681,64 +692,64 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="38.140625" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -768,7 +779,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -784,7 +795,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -795,22 +806,22 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BE+FE RipSites Actors Activity XLS export (in Team Productivity modal)
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40997A8F-8816-4FFE-8B19-128A95FF8AFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6512DB-6C37-4FD3-B36D-438297E779C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9915" yWindow="6690" windowWidth="36750" windowHeight="21030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23160" yWindow="9870" windowWidth="20850" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
     <sheet name="Synth" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$J$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$M$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>EWIN SERVICES</t>
   </si>
@@ -78,18 +78,9 @@
     <t>Total général</t>
   </si>
   <si>
-    <t>Étiquettes de colonnes</t>
-  </si>
-  <si>
     <t>Somme de Quantité</t>
   </si>
   <si>
-    <t>Total Somme de Quantité</t>
-  </si>
-  <si>
-    <t>Total Somme de Prix</t>
-  </si>
-  <si>
     <t>Somme de Prix</t>
   </si>
   <si>
@@ -97,6 +88,15 @@
   </si>
   <si>
     <t>Travail</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Activité</t>
   </si>
 </sst>
 </file>
@@ -169,46 +169,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -239,7 +284,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>309283</xdr:colOff>
+      <xdr:colOff>366433</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>150804</xdr:rowOff>
     </xdr:to>
@@ -284,15 +329,24 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43693.783743055559" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{4E7DB3FF-3921-4F05-9A1D-32673DE941C7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43730.749953472223" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{4E7DB3FF-3921-4F05-9A1D-32673DE941C7}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:J1009" sheet="EWIN"/>
   </cacheSource>
   <cacheFields count="10">
+    <cacheField name="Client" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Site" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Activité" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
     <cacheField name="Item" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Info" numFmtId="0">
+    <cacheField name="Info" numFmtId="164">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Code BPU" numFmtId="0">
@@ -300,27 +354,16 @@
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Quantité" numFmtId="0">
+    <cacheField name="Quantité" numFmtId="166">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Prix" numFmtId="164">
+    <cacheField name="Prix" numFmtId="165">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Quant. Tr." numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Travail" numFmtId="166">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Installé" numFmtId="165">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Equipe" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Date" numFmtId="0">
+    <cacheField name="Travail" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -337,22 +380,25 @@
   <r>
     <m/>
     <m/>
-    <x v="0"/>
-    <m/>
     <m/>
     <m/>
     <m/>
     <x v="0"/>
     <m/>
     <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86E8B809-2561-47F1-B5BD-247667BDDFCB}" name="Tableau croisé dynamique3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86E8B809-2561-47F1-B5BD-247667BDDFCB}" name="Tableau croisé dynamique3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -365,17 +411,9 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="2"/>
+    <field x="5"/>
   </rowFields>
   <rowItems count="2">
     <i>
@@ -385,28 +423,20 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="2">
-    <field x="7"/>
+  <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="2">
     <i>
       <x/>
-      <x/>
     </i>
-    <i r="1" i="1">
+    <i i="1">
       <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Somme de Quantité" fld="3" baseField="2" baseItem="0"/>
-    <dataField name="Somme de Prix" fld="4" baseField="2" baseItem="0"/>
+    <dataField name="Somme de Quantité" fld="6" baseField="2" baseItem="0"/>
+    <dataField name="Somme de Prix" fld="7" baseField="2" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -683,78 +713,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A1274-8C24-433A-8202-5D2FE710C049}">
-  <dimension ref="A2:J9"/>
+  <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="28"/>
+    <col min="12" max="12" width="32.5703125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I2" s="17"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I2" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="2"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="E9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="F9" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="G9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="H9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="L9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="M9" s="30" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A9:J243" xr:uid="{A0DF9817-DEF9-461E-807D-932DE473B341}"/>
+  <autoFilter ref="A9:M9" xr:uid="{EF10DD51-C0D6-4781-B96C-318E078678D0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -763,65 +806,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D00292-05A1-482C-9067-25F908AE77CB}">
-  <dimension ref="A3:E7"/>
+  <dimension ref="A3:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BE Polesites : Fix DICT Zip Archive (skip empty DICT data) + Fix Attachement XLS File
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6512DB-6C37-4FD3-B36D-438297E779C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B74A86-2D48-4E99-A594-3C5A511D04DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23160" yWindow="9870" windowWidth="20850" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16020" yWindow="1455" windowWidth="33045" windowHeight="29760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -103,10 +103,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -186,19 +185,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -216,7 +215,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -234,7 +233,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -329,11 +328,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43730.749953472223" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{4E7DB3FF-3921-4F05-9A1D-32673DE941C7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43773.487338541665" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{547A3FF2-F35D-4627-992E-9253879643D5}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A9:J1009" sheet="EWIN"/>
+    <worksheetSource ref="A9:M1009" sheet="EWIN"/>
   </cacheSource>
-  <cacheFields count="10">
+  <cacheFields count="13">
     <cacheField name="Client" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -346,24 +345,33 @@
     <cacheField name="Item" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Info" numFmtId="164">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Code BPU" numFmtId="0">
+    <cacheField name="Info" numFmtId="49">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Code BPU" numFmtId="49">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Quantité" numFmtId="166">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Prix" numFmtId="165">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Quant. Tr." numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Travail" numFmtId="0">
+    <cacheField name="Quantité" numFmtId="165">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Prix" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Quant. Tr." numFmtId="165">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Travail" numFmtId="2">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Installé" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Equipe" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="14">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -388,14 +396,17 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86E8B809-2561-47F1-B5BD-247667BDDFCB}" name="Tableau croisé dynamique3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B087FA2-9720-4D18-B236-C2E779F2C90F}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
+  <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -409,6 +420,9 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
@@ -715,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A1274-8C24-433A-8202-5D2FE710C049}">
   <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +823,7 @@
   <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BE RIP XLS Attachement : fix pivot table scope
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B74A86-2D48-4E99-A594-3C5A511D04DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1AF404-3302-4C10-8A09-27CCBFC6E123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16020" yWindow="1455" windowWidth="33045" windowHeight="29760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="2925" windowWidth="30840" windowHeight="25230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43773.487338541665" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{547A3FF2-F35D-4627-992E-9253879643D5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43783.810524884262" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{547A3FF2-F35D-4627-992E-9253879643D5}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:M1009" sheet="EWIN"/>
   </cacheSource>
@@ -404,7 +404,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B087FA2-9720-4D18-B236-C2E779F2C90F}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B087FA2-9720-4D18-B236-C2E779F2C90F}" name="Tableau croisé dynamique3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -729,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A1274-8C24-433A-8202-5D2FE710C049}">
   <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -823,7 +823,7 @@
   <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BE + FE Item : Add Billed status on item (applied to PoleSite)
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1AF404-3302-4C10-8A09-27CCBFC6E123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39A227F-D03F-4518-9032-062B1E5028E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="2925" windowWidth="30840" windowHeight="25230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="5520" windowWidth="37050" windowHeight="23565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
     <sheet name="Synth" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$M$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EWIN!$A$9:$O$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>EWIN SERVICES</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Prix</t>
   </si>
   <si>
-    <t>Installé</t>
-  </si>
-  <si>
     <t>Equipe</t>
   </si>
   <si>
@@ -97,6 +94,15 @@
   </si>
   <si>
     <t>Activité</t>
+  </si>
+  <si>
+    <t>Attach.</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>Etat</t>
   </si>
 </sst>
 </file>
@@ -168,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -253,6 +259,12 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -328,7 +340,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43783.810524884262" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{547A3FF2-F35D-4627-992E-9253879643D5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43832.900077777776" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{547A3FF2-F35D-4627-992E-9253879643D5}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:M1009" sheet="EWIN"/>
   </cacheSource>
@@ -404,7 +416,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B087FA2-9720-4D18-B236-C2E779F2C90F}" name="Tableau croisé dynamique3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B087FA2-9720-4D18-B236-C2E779F2C90F}" name="Tableau croisé dynamique3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -727,7 +739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A1274-8C24-433A-8202-5D2FE710C049}">
-  <dimension ref="A2:M9"/>
+  <dimension ref="A2:O9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -745,15 +757,16 @@
     <col min="8" max="8" width="14.7109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="10" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="28"/>
+    <col min="11" max="11" width="14.7109375" style="28" customWidth="1"/>
     <col min="12" max="12" width="32.5703125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="29" customWidth="1"/>
+    <col min="13" max="14" width="13.7109375" style="29" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I2" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
@@ -769,15 +782,15 @@
       <c r="I7" s="18"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>2</v>
@@ -795,23 +808,29 @@
         <v>6</v>
       </c>
       <c r="I9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="25" t="s">
-        <v>16</v>
-      </c>
       <c r="K9" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="M9" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="30" t="s">
-        <v>9</v>
+      <c r="N9" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A9:M9" xr:uid="{EF10DD51-C0D6-4781-B96C-318E078678D0}"/>
+  <autoFilter ref="A9:O9" xr:uid="{5143A540-6C08-4DD4-98F1-81FEC95790D3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -837,25 +856,25 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>

</xml_diff>

<commit_message>
BE ATTACHEMENT _RIPREF_.xlsx : Update PivotTable range
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39A227F-D03F-4518-9032-062B1E5028E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9144377-1598-4887-B85A-A75FE8B12901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="5520" windowWidth="37050" windowHeight="23565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="4920" windowWidth="43500" windowHeight="23940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="27" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -340,11 +340,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43832.900077777776" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{547A3FF2-F35D-4627-992E-9253879643D5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent" refreshedDate="43834.812697222224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{3266A5BF-E6D9-4E1B-88D7-2C09C575FFD5}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A9:M1009" sheet="EWIN"/>
+    <worksheetSource ref="A9:N1009" sheet="EWIN"/>
   </cacheSource>
-  <cacheFields count="13">
+  <cacheFields count="14">
     <cacheField name="Client" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -377,13 +377,16 @@
     <cacheField name="Travail" numFmtId="2">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Installé" numFmtId="0">
+    <cacheField name="Etat" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Equipe" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Date" numFmtId="14">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Attach." numFmtId="14">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -411,14 +414,15 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B087FA2-9720-4D18-B236-C2E779F2C90F}" name="Tableau croisé dynamique3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62D5147D-D99E-4E8C-87FD-4A3B6A906410}" name="Tableau croisé dynamique3" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
+  <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -432,6 +436,7 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -842,7 +847,7 @@
   <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BE ATTACHEMENT _RIPREF_.xlsx : Update PivotTable range and update at open time
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9144377-1598-4887-B85A-A75FE8B12901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97304C0E-C8FD-47BF-B6D8-A10E98DC7E7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4920" windowWidth="43500" windowHeight="23940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="5130" windowWidth="49995" windowHeight="21885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="27" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Laurent" refreshedDate="43834.812697222224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{3266A5BF-E6D9-4E1B-88D7-2C09C575FFD5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43834.812697222224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{3266A5BF-E6D9-4E1B-88D7-2C09C575FFD5}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:N1009" sheet="EWIN"/>
   </cacheSource>
@@ -420,7 +420,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62D5147D-D99E-4E8C-87FD-4A3B6A906410}" name="Tableau croisé dynamique3" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62D5147D-D99E-4E8C-87FD-4A3B6A906410}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>

</xml_diff>

<commit_message>
BE Rip Attachement : Extend PivotTable Scope
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
+++ b/Ressources/DocTemplates/ATTACHEMENT _RIPREF_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97304C0E-C8FD-47BF-B6D8-A10E98DC7E7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00746F57-E319-4178-8EA2-AF4015DAC0C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="5130" windowWidth="49995" windowHeight="21885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7515" yWindow="3060" windowWidth="43140" windowHeight="23865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWIN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -340,9 +340,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43834.812697222224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{3266A5BF-E6D9-4E1B-88D7-2C09C575FFD5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Laurent" refreshedDate="43892.754185069447" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{BD7A572F-EE0A-4424-8E08-3877826E8AE9}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A9:N1009" sheet="EWIN"/>
+    <worksheetSource ref="A9:N2009" sheet="EWIN"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="Client" numFmtId="0">
@@ -420,7 +420,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62D5147D-D99E-4E8C-87FD-4A3B6A906410}" name="Tableau croisé dynamique3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BEACAA36-E6DC-4B18-9019-B0C06F6B4081}" name="Tableau croisé dynamique3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>

</xml_diff>